<commit_message>
Updated DB and routes
</commit_message>
<xml_diff>
--- a/DB_Diagram.xlsx
+++ b/DB_Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/makikovaughan/bc/homework/amazonisles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF19ED-01EF-1B46-9FAB-F6A6E9D45A1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0368F639-1A25-054A-BBFA-0BD45F2A9EC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{EF66BB67-DC15-8F4B-B1A7-2742186865A0}"/>
   </bookViews>
@@ -1514,7 +1514,7 @@
                             <a:p>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000"/>
-                                <a:t>measurement:</a:t>
+                                <a:t>measurement	:</a:t>
                               </a:r>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000" baseline="0"/>

</xml_diff>

<commit_message>
Some of my works were deleted
</commit_message>
<xml_diff>
--- a/DB_Diagram.xlsx
+++ b/DB_Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/makikovaughan/bc/homework/amazonisles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0368F639-1A25-054A-BBFA-0BD45F2A9EC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65C91B8-5B51-C246-9721-8D73A2942931}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{EF66BB67-DC15-8F4B-B1A7-2742186865A0}"/>
   </bookViews>
@@ -549,56 +549,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>325966</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>8466</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>723899</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>21166</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="114" name="Straight Connector 113">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04C7519D-5332-8D44-80DA-60E9F2B815C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11942233" y="6307666"/>
-          <a:ext cx="3716866" cy="12700"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>220134</xdr:colOff>
       <xdr:row>23</xdr:row>
@@ -700,9 +650,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
@@ -723,10 +673,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5435600" y="11557000"/>
-          <a:ext cx="9829800" cy="5029200"/>
-          <a:chOff x="5410200" y="11557000"/>
-          <a:chExt cx="9779000" cy="5029200"/>
+          <a:off x="5334000" y="11040533"/>
+          <a:ext cx="9931400" cy="5545667"/>
+          <a:chOff x="5309125" y="11040533"/>
+          <a:chExt cx="9880075" cy="5545667"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -923,9 +873,9 @@
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="5410200" y="11557000"/>
-            <a:ext cx="5956300" cy="38100"/>
+          <a:xfrm>
+            <a:off x="5309125" y="11040533"/>
+            <a:ext cx="6047651" cy="50800"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -959,12 +909,12 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm rot="16200000" flipH="1">
-            <a:off x="10693400" y="12255500"/>
-            <a:ext cx="2324100" cy="927100"/>
+            <a:off x="10434626" y="11996725"/>
+            <a:ext cx="2772833" cy="995916"/>
           </a:xfrm>
           <a:prstGeom prst="bentConnector3">
             <a:avLst>
-              <a:gd name="adj1" fmla="val 99180"/>
+              <a:gd name="adj1" fmla="val 50000"/>
             </a:avLst>
           </a:prstGeom>
           <a:ln>
@@ -1097,15 +1047,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>355599</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:colOff>50801</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>131233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>389468</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>33869</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>131234</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1120,10 +1070,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="355599" y="723899"/>
-          <a:ext cx="15798802" cy="16052801"/>
-          <a:chOff x="355599" y="723899"/>
-          <a:chExt cx="15798802" cy="16052801"/>
+          <a:off x="50801" y="131233"/>
+          <a:ext cx="15748001" cy="16052801"/>
+          <a:chOff x="406400" y="723899"/>
+          <a:chExt cx="15748001" cy="16052801"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -1139,10 +1089,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="355599" y="723899"/>
-            <a:ext cx="15273868" cy="16052801"/>
-            <a:chOff x="355599" y="723899"/>
-            <a:chExt cx="15273868" cy="16052801"/>
+            <a:off x="406400" y="723899"/>
+            <a:ext cx="14765866" cy="16052801"/>
+            <a:chOff x="406400" y="723899"/>
+            <a:chExt cx="14765866" cy="16052801"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:grpSp>
@@ -1158,10 +1108,10 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="355599" y="723899"/>
-              <a:ext cx="15273868" cy="16052801"/>
-              <a:chOff x="355533" y="723899"/>
-              <a:chExt cx="15194207" cy="16052801"/>
+              <a:off x="406400" y="723899"/>
+              <a:ext cx="14765866" cy="16052801"/>
+              <a:chOff x="406069" y="723899"/>
+              <a:chExt cx="14688855" cy="16052801"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:grpSp>
@@ -1177,10 +1127,10 @@
             </xdr:nvGrpSpPr>
             <xdr:grpSpPr>
               <a:xfrm>
-                <a:off x="355533" y="723899"/>
-                <a:ext cx="15194207" cy="13974233"/>
-                <a:chOff x="355533" y="723899"/>
-                <a:chExt cx="15194207" cy="13974233"/>
+                <a:off x="406069" y="723899"/>
+                <a:ext cx="14688855" cy="13974233"/>
+                <a:chOff x="406069" y="723899"/>
+                <a:chExt cx="14688855" cy="13974233"/>
               </a:xfrm>
             </xdr:grpSpPr>
             <xdr:grpSp>
@@ -1197,17 +1147,17 @@
               <xdr:grpSpPr>
                 <a:xfrm>
                   <a:off x="1096715" y="723899"/>
-                  <a:ext cx="14453025" cy="13974233"/>
+                  <a:ext cx="13998209" cy="13974233"/>
                   <a:chOff x="1096715" y="723899"/>
-                  <a:chExt cx="14453025" cy="13974233"/>
+                  <a:chExt cx="13998209" cy="13974233"/>
                 </a:xfrm>
               </xdr:grpSpPr>
               <xdr:grpSp>
                 <xdr:nvGrpSpPr>
-                  <xdr:cNvPr id="118" name="Group 117">
+                  <xdr:cNvPr id="112" name="Group 111">
                     <a:extLst>
                       <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89957DB5-5BA7-D44E-AEA8-4544593C67BB}"/>
+                        <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A04B77-F46E-7F49-9928-545F920A6A41}"/>
                       </a:ext>
                     </a:extLst>
                   </xdr:cNvPr>
@@ -1216,17 +1166,17 @@
                 <xdr:grpSpPr>
                   <a:xfrm>
                     <a:off x="1562100" y="723899"/>
-                    <a:ext cx="13987640" cy="13974233"/>
+                    <a:ext cx="13532824" cy="13974233"/>
                     <a:chOff x="1562100" y="723899"/>
-                    <a:chExt cx="13987640" cy="13974233"/>
+                    <a:chExt cx="13532824" cy="13974233"/>
                   </a:xfrm>
                 </xdr:grpSpPr>
                 <xdr:grpSp>
                   <xdr:nvGrpSpPr>
-                    <xdr:cNvPr id="112" name="Group 111">
+                    <xdr:cNvPr id="93" name="Group 92">
                       <a:extLst>
                         <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A04B77-F46E-7F49-9928-545F920A6A41}"/>
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC811917-03FD-674E-8741-A3F8F94B4F86}"/>
                         </a:ext>
                       </a:extLst>
                     </xdr:cNvPr>
@@ -1235,17 +1185,17 @@
                   <xdr:grpSpPr>
                     <a:xfrm>
                       <a:off x="1562100" y="723899"/>
-                      <a:ext cx="13487401" cy="13974233"/>
+                      <a:ext cx="13532824" cy="10744201"/>
                       <a:chOff x="1562100" y="723899"/>
-                      <a:chExt cx="13487401" cy="13974233"/>
+                      <a:chExt cx="13532824" cy="10744201"/>
                     </a:xfrm>
                   </xdr:grpSpPr>
                   <xdr:grpSp>
                     <xdr:nvGrpSpPr>
-                      <xdr:cNvPr id="93" name="Group 92">
+                      <xdr:cNvPr id="67" name="Group 66">
                         <a:extLst>
                           <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC811917-03FD-674E-8741-A3F8F94B4F86}"/>
+                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86AA123E-771A-4F48-8428-9BFA8C258350}"/>
                           </a:ext>
                         </a:extLst>
                       </xdr:cNvPr>
@@ -1254,17 +1204,17 @@
                     <xdr:grpSpPr>
                       <a:xfrm>
                         <a:off x="1562100" y="723899"/>
-                        <a:ext cx="13487401" cy="10744201"/>
+                        <a:ext cx="13532824" cy="10744201"/>
                         <a:chOff x="1562100" y="723899"/>
-                        <a:chExt cx="13487401" cy="10744201"/>
+                        <a:chExt cx="13532824" cy="10744201"/>
                       </a:xfrm>
                     </xdr:grpSpPr>
                     <xdr:grpSp>
                       <xdr:nvGrpSpPr>
-                        <xdr:cNvPr id="67" name="Group 66">
+                        <xdr:cNvPr id="10" name="Group 9">
                           <a:extLst>
                             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86AA123E-771A-4F48-8428-9BFA8C258350}"/>
+                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5232C7F-3388-8D44-B3F9-07A46A15A2FC}"/>
                             </a:ext>
                           </a:extLst>
                         </xdr:cNvPr>
@@ -1273,17 +1223,17 @@
                       <xdr:grpSpPr>
                         <a:xfrm>
                           <a:off x="1562100" y="723899"/>
-                          <a:ext cx="13487401" cy="10744201"/>
+                          <a:ext cx="3352800" cy="5846234"/>
                           <a:chOff x="1562100" y="723899"/>
-                          <a:chExt cx="13487401" cy="10744201"/>
+                          <a:chExt cx="3352800" cy="5846234"/>
                         </a:xfrm>
                       </xdr:grpSpPr>
                       <xdr:grpSp>
                         <xdr:nvGrpSpPr>
-                          <xdr:cNvPr id="10" name="Group 9">
+                          <xdr:cNvPr id="6" name="Group 5">
                             <a:extLst>
                               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5232C7F-3388-8D44-B3F9-07A46A15A2FC}"/>
+                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C0A58BE-690F-4243-AD13-90163242C809}"/>
                               </a:ext>
                             </a:extLst>
                           </xdr:cNvPr>
@@ -1297,12 +1247,288 @@
                             <a:chExt cx="3352800" cy="5846234"/>
                           </a:xfrm>
                         </xdr:grpSpPr>
+                        <xdr:sp macro="" textlink="">
+                          <xdr:nvSpPr>
+                            <xdr:cNvPr id="3" name="Process 2">
+                              <a:extLst>
+                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3D0CA4-FC4A-0F48-9239-24DEAA2CC5A6}"/>
+                                </a:ext>
+                              </a:extLst>
+                            </xdr:cNvPr>
+                            <xdr:cNvSpPr/>
+                          </xdr:nvSpPr>
+                          <xdr:spPr>
+                            <a:xfrm>
+                              <a:off x="1587500" y="723899"/>
+                              <a:ext cx="3314700" cy="5846234"/>
+                            </a:xfrm>
+                            <a:prstGeom prst="flowChartProcess">
+                              <a:avLst/>
+                            </a:prstGeom>
+                          </xdr:spPr>
+                          <xdr:style>
+                            <a:lnRef idx="2">
+                              <a:schemeClr val="accent6"/>
+                            </a:lnRef>
+                            <a:fillRef idx="1">
+                              <a:schemeClr val="lt1"/>
+                            </a:fillRef>
+                            <a:effectRef idx="0">
+                              <a:schemeClr val="accent6"/>
+                            </a:effectRef>
+                            <a:fontRef idx="minor">
+                              <a:schemeClr val="dk1"/>
+                            </a:fontRef>
+                          </xdr:style>
+                          <xdr:txBody>
+                            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                            <a:lstStyle/>
+                            <a:p>
+                              <a:pPr algn="l"/>
+                              <a:endParaRPr lang="en-US" sz="1100"/>
+                            </a:p>
+                            <a:p>
+                              <a:pPr algn="l"/>
+                              <a:r>
+                                <a:rPr lang="en-US" sz="1800"/>
+                                <a:t>	</a:t>
+                              </a:r>
+                            </a:p>
+                          </xdr:txBody>
+                        </xdr:sp>
+                        <xdr:cxnSp macro="">
+                          <xdr:nvCxnSpPr>
+                            <xdr:cNvPr id="5" name="Straight Connector 4">
+                              <a:extLst>
+                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{908C480E-3DC5-9F4B-8F77-0ED7CDAFFDD9}"/>
+                                </a:ext>
+                              </a:extLst>
+                            </xdr:cNvPr>
+                            <xdr:cNvCxnSpPr/>
+                          </xdr:nvCxnSpPr>
+                          <xdr:spPr>
+                            <a:xfrm>
+                              <a:off x="1562100" y="1587500"/>
+                              <a:ext cx="3352800" cy="0"/>
+                            </a:xfrm>
+                            <a:prstGeom prst="line">
+                              <a:avLst/>
+                            </a:prstGeom>
+                          </xdr:spPr>
+                          <xdr:style>
+                            <a:lnRef idx="1">
+                              <a:schemeClr val="accent1"/>
+                            </a:lnRef>
+                            <a:fillRef idx="0">
+                              <a:schemeClr val="accent1"/>
+                            </a:fillRef>
+                            <a:effectRef idx="0">
+                              <a:schemeClr val="accent1"/>
+                            </a:effectRef>
+                            <a:fontRef idx="minor">
+                              <a:schemeClr val="tx1"/>
+                            </a:fontRef>
+                          </xdr:style>
+                        </xdr:cxnSp>
+                      </xdr:grpSp>
+                      <xdr:sp macro="" textlink="">
+                        <xdr:nvSpPr>
+                          <xdr:cNvPr id="8" name="TextBox 7">
+                            <a:extLst>
+                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D058A20-4E0E-DF44-98D7-62652831342A}"/>
+                              </a:ext>
+                            </a:extLst>
+                          </xdr:cNvPr>
+                          <xdr:cNvSpPr txBox="1"/>
+                        </xdr:nvSpPr>
+                        <xdr:spPr>
+                          <a:xfrm>
+                            <a:off x="2298700" y="939800"/>
+                            <a:ext cx="2006600" cy="482600"/>
+                          </a:xfrm>
+                          <a:prstGeom prst="rect">
+                            <a:avLst/>
+                          </a:prstGeom>
+                          <a:solidFill>
+                            <a:schemeClr val="lt1"/>
+                          </a:solidFill>
+                          <a:ln w="9525" cmpd="sng">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:shade val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                        </xdr:spPr>
+                        <xdr:style>
+                          <a:lnRef idx="0">
+                            <a:scrgbClr r="0" g="0" b="0"/>
+                          </a:lnRef>
+                          <a:fillRef idx="0">
+                            <a:scrgbClr r="0" g="0" b="0"/>
+                          </a:fillRef>
+                          <a:effectRef idx="0">
+                            <a:scrgbClr r="0" g="0" b="0"/>
+                          </a:effectRef>
+                          <a:fontRef idx="minor">
+                            <a:schemeClr val="dk1"/>
+                          </a:fontRef>
+                        </xdr:style>
+                        <xdr:txBody>
+                          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                          <a:lstStyle/>
+                          <a:p>
+                            <a:pPr algn="ctr"/>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2400"/>
+                              <a:t>Clients</a:t>
+                            </a:r>
+                          </a:p>
+                        </xdr:txBody>
+                      </xdr:sp>
+                      <xdr:sp macro="" textlink="">
+                        <xdr:nvSpPr>
+                          <xdr:cNvPr id="9" name="TextBox 8">
+                            <a:extLst>
+                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9AFFB4A-114C-C24E-B630-F2571D1D925D}"/>
+                              </a:ext>
+                            </a:extLst>
+                          </xdr:cNvPr>
+                          <xdr:cNvSpPr txBox="1"/>
+                        </xdr:nvSpPr>
+                        <xdr:spPr>
+                          <a:xfrm>
+                            <a:off x="1854200" y="1866898"/>
+                            <a:ext cx="2870200" cy="4432302"/>
+                          </a:xfrm>
+                          <a:prstGeom prst="rect">
+                            <a:avLst/>
+                          </a:prstGeom>
+                          <a:solidFill>
+                            <a:schemeClr val="lt1"/>
+                          </a:solidFill>
+                          <a:ln w="9525" cmpd="sng">
+                            <a:solidFill>
+                              <a:schemeClr val="lt1">
+                                <a:shade val="50000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                        </xdr:spPr>
+                        <xdr:style>
+                          <a:lnRef idx="0">
+                            <a:scrgbClr r="0" g="0" b="0"/>
+                          </a:lnRef>
+                          <a:fillRef idx="0">
+                            <a:scrgbClr r="0" g="0" b="0"/>
+                          </a:fillRef>
+                          <a:effectRef idx="0">
+                            <a:scrgbClr r="0" g="0" b="0"/>
+                          </a:effectRef>
+                          <a:fontRef idx="minor">
+                            <a:schemeClr val="dk1"/>
+                          </a:fontRef>
+                        </xdr:style>
+                        <xdr:txBody>
+                          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+                          <a:lstStyle/>
+                          <a:p>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000"/>
+                              <a:t>measurement	:</a:t>
+                            </a:r>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                              <a:t> (</a:t>
+                            </a:r>
+                          </a:p>
+                          <a:p>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                              <a:t>   weist: Number</a:t>
+                            </a:r>
+                          </a:p>
+                          <a:p>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                              <a:t>   bust: Number</a:t>
+                            </a:r>
+                          </a:p>
+                          <a:p>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                              <a:t>   arm_length: Number</a:t>
+                            </a:r>
+                          </a:p>
+                          <a:p>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                              <a:t>   leg_length: Number</a:t>
+                            </a:r>
+                          </a:p>
+                          <a:p>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                              <a:t>)</a:t>
+                            </a:r>
+                          </a:p>
+                          <a:p>
+                            <a:r>
+                              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                              <a:t>orders: FK(Array)</a:t>
+                            </a:r>
+                          </a:p>
+                        </xdr:txBody>
+                      </xdr:sp>
+                    </xdr:grpSp>
+                    <xdr:grpSp>
+                      <xdr:nvGrpSpPr>
+                        <xdr:cNvPr id="59" name="Group 58">
+                          <a:extLst>
+                            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE38A0E4-956E-8048-B6CF-6CB398E9DCB7}"/>
+                            </a:ext>
+                          </a:extLst>
+                        </xdr:cNvPr>
+                        <xdr:cNvGrpSpPr/>
+                      </xdr:nvGrpSpPr>
+                      <xdr:grpSpPr>
+                        <a:xfrm>
+                          <a:off x="8053706" y="1155700"/>
+                          <a:ext cx="7041218" cy="10312400"/>
+                          <a:chOff x="8536306" y="825500"/>
+                          <a:chExt cx="7041218" cy="10312400"/>
+                        </a:xfrm>
+                      </xdr:grpSpPr>
+                      <xdr:grpSp>
+                        <xdr:nvGrpSpPr>
+                          <xdr:cNvPr id="11" name="Group 10">
+                            <a:extLst>
+                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B9CF36B-7C68-0143-A73D-E8FA7F4DD114}"/>
+                              </a:ext>
+                            </a:extLst>
+                          </xdr:cNvPr>
+                          <xdr:cNvGrpSpPr/>
+                        </xdr:nvGrpSpPr>
+                        <xdr:grpSpPr>
+                          <a:xfrm>
+                            <a:off x="10363200" y="825500"/>
+                            <a:ext cx="3563513" cy="5702300"/>
+                            <a:chOff x="1562100" y="723900"/>
+                            <a:chExt cx="3563513" cy="5702300"/>
+                          </a:xfrm>
+                        </xdr:grpSpPr>
                         <xdr:grpSp>
                           <xdr:nvGrpSpPr>
-                            <xdr:cNvPr id="6" name="Group 5">
+                            <xdr:cNvPr id="12" name="Group 11">
                               <a:extLst>
                                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C0A58BE-690F-4243-AD13-90163242C809}"/>
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27402B51-87F8-F14A-984A-00F5F7BDB21D}"/>
                                 </a:ext>
                               </a:extLst>
                             </xdr:cNvPr>
@@ -1310,18 +1536,18 @@
                           </xdr:nvGrpSpPr>
                           <xdr:grpSpPr>
                             <a:xfrm>
-                              <a:off x="1562100" y="723899"/>
-                              <a:ext cx="3352800" cy="5846234"/>
-                              <a:chOff x="1562100" y="723899"/>
-                              <a:chExt cx="3352800" cy="5846234"/>
+                              <a:off x="1562100" y="723900"/>
+                              <a:ext cx="3563513" cy="5702300"/>
+                              <a:chOff x="1562100" y="723900"/>
+                              <a:chExt cx="3563513" cy="5702300"/>
                             </a:xfrm>
                           </xdr:grpSpPr>
                           <xdr:sp macro="" textlink="">
                             <xdr:nvSpPr>
-                              <xdr:cNvPr id="3" name="Process 2">
+                              <xdr:cNvPr id="15" name="Process 14">
                                 <a:extLst>
                                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3D0CA4-FC4A-0F48-9239-24DEAA2CC5A6}"/>
+                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D869B504-945F-7B49-B644-07555770576A}"/>
                                   </a:ext>
                                 </a:extLst>
                               </xdr:cNvPr>
@@ -1329,8 +1555,8 @@
                             </xdr:nvSpPr>
                             <xdr:spPr>
                               <a:xfrm>
-                                <a:off x="1587500" y="723899"/>
-                                <a:ext cx="3314700" cy="5846234"/>
+                                <a:off x="1587499" y="723900"/>
+                                <a:ext cx="3505695" cy="5702300"/>
                               </a:xfrm>
                               <a:prstGeom prst="flowChartProcess">
                                 <a:avLst/>
@@ -1368,10 +1594,10 @@
                           </xdr:sp>
                           <xdr:cxnSp macro="">
                             <xdr:nvCxnSpPr>
-                              <xdr:cNvPr id="5" name="Straight Connector 4">
+                              <xdr:cNvPr id="16" name="Straight Connector 15">
                                 <a:extLst>
                                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{908C480E-3DC5-9F4B-8F77-0ED7CDAFFDD9}"/>
+                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7551C24-9DE9-134B-8100-BBACF07BBC9B}"/>
                                   </a:ext>
                                 </a:extLst>
                               </xdr:cNvPr>
@@ -1380,7 +1606,7 @@
                             <xdr:spPr>
                               <a:xfrm>
                                 <a:off x="1562100" y="1587500"/>
-                                <a:ext cx="3352800" cy="0"/>
+                                <a:ext cx="3563513" cy="29633"/>
                               </a:xfrm>
                               <a:prstGeom prst="line">
                                 <a:avLst/>
@@ -1404,10 +1630,10 @@
                         </xdr:grpSp>
                         <xdr:sp macro="" textlink="">
                           <xdr:nvSpPr>
-                            <xdr:cNvPr id="8" name="TextBox 7">
+                            <xdr:cNvPr id="13" name="TextBox 12">
                               <a:extLst>
                                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D058A20-4E0E-DF44-98D7-62652831342A}"/>
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF912565-9D52-9044-9609-A04D56ECF7F7}"/>
                                 </a:ext>
                               </a:extLst>
                             </xdr:cNvPr>
@@ -1453,17 +1679,17 @@
                               <a:pPr algn="ctr"/>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2400"/>
-                                <a:t>Clients</a:t>
+                                <a:t>Providers</a:t>
                               </a:r>
                             </a:p>
                           </xdr:txBody>
                         </xdr:sp>
                         <xdr:sp macro="" textlink="">
                           <xdr:nvSpPr>
-                            <xdr:cNvPr id="9" name="TextBox 8">
+                            <xdr:cNvPr id="14" name="TextBox 13">
                               <a:extLst>
                                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9AFFB4A-114C-C24E-B630-F2571D1D925D}"/>
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F50ADC-0BA1-D944-AA3E-CA1B19225CC0}"/>
                                 </a:ext>
                               </a:extLst>
                             </xdr:cNvPr>
@@ -1471,8 +1697,262 @@
                           </xdr:nvSpPr>
                           <xdr:spPr>
                             <a:xfrm>
-                              <a:off x="1854200" y="1866898"/>
-                              <a:ext cx="2870200" cy="4432302"/>
+                              <a:off x="1854200" y="1866899"/>
+                              <a:ext cx="3018738" cy="4389968"/>
+                            </a:xfrm>
+                            <a:prstGeom prst="rect">
+                              <a:avLst/>
+                            </a:prstGeom>
+                            <a:solidFill>
+                              <a:schemeClr val="lt1"/>
+                            </a:solidFill>
+                            <a:ln w="9525" cmpd="sng">
+                              <a:solidFill>
+                                <a:schemeClr val="lt1">
+                                  <a:shade val="50000"/>
+                                </a:schemeClr>
+                              </a:solidFill>
+                            </a:ln>
+                          </xdr:spPr>
+                          <xdr:style>
+                            <a:lnRef idx="0">
+                              <a:scrgbClr r="0" g="0" b="0"/>
+                            </a:lnRef>
+                            <a:fillRef idx="0">
+                              <a:scrgbClr r="0" g="0" b="0"/>
+                            </a:fillRef>
+                            <a:effectRef idx="0">
+                              <a:scrgbClr r="0" g="0" b="0"/>
+                            </a:effectRef>
+                            <a:fontRef idx="minor">
+                              <a:schemeClr val="dk1"/>
+                            </a:fontRef>
+                          </xdr:style>
+                          <xdr:txBody>
+                            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+                            <a:lstStyle/>
+                            <a:p>
+                              <a:r>
+                                <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                                <a:t>demo: String(web link)</a:t>
+                              </a:r>
+                            </a:p>
+                            <a:p>
+                              <a:r>
+                                <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                                <a:t>photo: String(Web link)</a:t>
+                              </a:r>
+                            </a:p>
+                            <a:p>
+                              <a:r>
+                                <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                                <a:t>category: String</a:t>
+                              </a:r>
+                            </a:p>
+                            <a:p>
+                              <a:r>
+                                <a:rPr lang="en-US" sz="2000"/>
+                                <a:t>orders: FK (Array)</a:t>
+                              </a:r>
+                            </a:p>
+                          </xdr:txBody>
+                        </xdr:sp>
+                      </xdr:grpSp>
+                      <xdr:grpSp>
+                        <xdr:nvGrpSpPr>
+                          <xdr:cNvPr id="17" name="Group 16">
+                            <a:extLst>
+                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C078A5B-E556-E14B-ACDE-5386842E7585}"/>
+                              </a:ext>
+                            </a:extLst>
+                          </xdr:cNvPr>
+                          <xdr:cNvGrpSpPr/>
+                        </xdr:nvGrpSpPr>
+                        <xdr:grpSpPr>
+                          <a:xfrm>
+                            <a:off x="10473355" y="7023100"/>
+                            <a:ext cx="3352800" cy="4114800"/>
+                            <a:chOff x="1545255" y="1739900"/>
+                            <a:chExt cx="3352800" cy="4114800"/>
+                          </a:xfrm>
+                        </xdr:grpSpPr>
+                        <xdr:grpSp>
+                          <xdr:nvGrpSpPr>
+                            <xdr:cNvPr id="18" name="Group 17">
+                              <a:extLst>
+                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{550BD863-8F60-A34F-954F-643FF9ED6B08}"/>
+                                </a:ext>
+                              </a:extLst>
+                            </xdr:cNvPr>
+                            <xdr:cNvGrpSpPr/>
+                          </xdr:nvGrpSpPr>
+                          <xdr:grpSpPr>
+                            <a:xfrm>
+                              <a:off x="1545255" y="1739900"/>
+                              <a:ext cx="3352800" cy="4114800"/>
+                              <a:chOff x="1545255" y="1739900"/>
+                              <a:chExt cx="3352800" cy="4114800"/>
+                            </a:xfrm>
+                          </xdr:grpSpPr>
+                          <xdr:sp macro="" textlink="">
+                            <xdr:nvSpPr>
+                              <xdr:cNvPr id="21" name="Process 20">
+                                <a:extLst>
+                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53172DB7-8D2A-4F4F-AD26-947E88B3F7BB}"/>
+                                  </a:ext>
+                                </a:extLst>
+                              </xdr:cNvPr>
+                              <xdr:cNvSpPr/>
+                            </xdr:nvSpPr>
+                            <xdr:spPr>
+                              <a:xfrm>
+                                <a:off x="1570655" y="1739900"/>
+                                <a:ext cx="3314700" cy="4114800"/>
+                              </a:xfrm>
+                              <a:prstGeom prst="flowChartProcess">
+                                <a:avLst/>
+                              </a:prstGeom>
+                            </xdr:spPr>
+                            <xdr:style>
+                              <a:lnRef idx="2">
+                                <a:schemeClr val="accent6"/>
+                              </a:lnRef>
+                              <a:fillRef idx="1">
+                                <a:schemeClr val="lt1"/>
+                              </a:fillRef>
+                              <a:effectRef idx="0">
+                                <a:schemeClr val="accent6"/>
+                              </a:effectRef>
+                              <a:fontRef idx="minor">
+                                <a:schemeClr val="dk1"/>
+                              </a:fontRef>
+                            </xdr:style>
+                            <xdr:txBody>
+                              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                              <a:lstStyle/>
+                              <a:p>
+                                <a:pPr algn="l"/>
+                                <a:endParaRPr lang="en-US" sz="1100"/>
+                              </a:p>
+                              <a:p>
+                                <a:pPr algn="l"/>
+                                <a:r>
+                                  <a:rPr lang="en-US" sz="1800"/>
+                                  <a:t>	</a:t>
+                                </a:r>
+                              </a:p>
+                            </xdr:txBody>
+                          </xdr:sp>
+                          <xdr:cxnSp macro="">
+                            <xdr:nvCxnSpPr>
+                              <xdr:cNvPr id="22" name="Straight Connector 21">
+                                <a:extLst>
+                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61B48F51-0827-B242-852D-17948613BE1A}"/>
+                                  </a:ext>
+                                </a:extLst>
+                              </xdr:cNvPr>
+                              <xdr:cNvCxnSpPr/>
+                            </xdr:nvCxnSpPr>
+                            <xdr:spPr>
+                              <a:xfrm>
+                                <a:off x="1545255" y="2603500"/>
+                                <a:ext cx="3352800" cy="0"/>
+                              </a:xfrm>
+                              <a:prstGeom prst="line">
+                                <a:avLst/>
+                              </a:prstGeom>
+                            </xdr:spPr>
+                            <xdr:style>
+                              <a:lnRef idx="1">
+                                <a:schemeClr val="accent1"/>
+                              </a:lnRef>
+                              <a:fillRef idx="0">
+                                <a:schemeClr val="accent1"/>
+                              </a:fillRef>
+                              <a:effectRef idx="0">
+                                <a:schemeClr val="accent1"/>
+                              </a:effectRef>
+                              <a:fontRef idx="minor">
+                                <a:schemeClr val="tx1"/>
+                              </a:fontRef>
+                            </xdr:style>
+                          </xdr:cxnSp>
+                        </xdr:grpSp>
+                        <xdr:sp macro="" textlink="">
+                          <xdr:nvSpPr>
+                            <xdr:cNvPr id="19" name="TextBox 18">
+                              <a:extLst>
+                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF63E278-3D33-0E4B-A98E-2865211A52CF}"/>
+                                </a:ext>
+                              </a:extLst>
+                            </xdr:cNvPr>
+                            <xdr:cNvSpPr txBox="1"/>
+                          </xdr:nvSpPr>
+                          <xdr:spPr>
+                            <a:xfrm>
+                              <a:off x="2281855" y="1955800"/>
+                              <a:ext cx="2006600" cy="482600"/>
+                            </a:xfrm>
+                            <a:prstGeom prst="rect">
+                              <a:avLst/>
+                            </a:prstGeom>
+                            <a:solidFill>
+                              <a:schemeClr val="lt1"/>
+                            </a:solidFill>
+                            <a:ln w="9525" cmpd="sng">
+                              <a:solidFill>
+                                <a:schemeClr val="lt1">
+                                  <a:shade val="50000"/>
+                                </a:schemeClr>
+                              </a:solidFill>
+                            </a:ln>
+                          </xdr:spPr>
+                          <xdr:style>
+                            <a:lnRef idx="0">
+                              <a:scrgbClr r="0" g="0" b="0"/>
+                            </a:lnRef>
+                            <a:fillRef idx="0">
+                              <a:scrgbClr r="0" g="0" b="0"/>
+                            </a:fillRef>
+                            <a:effectRef idx="0">
+                              <a:scrgbClr r="0" g="0" b="0"/>
+                            </a:effectRef>
+                            <a:fontRef idx="minor">
+                              <a:schemeClr val="dk1"/>
+                            </a:fontRef>
+                          </xdr:style>
+                          <xdr:txBody>
+                            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                            <a:lstStyle/>
+                            <a:p>
+                              <a:pPr algn="ctr"/>
+                              <a:r>
+                                <a:rPr lang="en-US" sz="2400"/>
+                                <a:t>Reviews</a:t>
+                              </a:r>
+                            </a:p>
+                          </xdr:txBody>
+                        </xdr:sp>
+                        <xdr:sp macro="" textlink="">
+                          <xdr:nvSpPr>
+                            <xdr:cNvPr id="20" name="TextBox 19">
+                              <a:extLst>
+                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A50AE9-0294-2B4C-9FC2-2DBA40869262}"/>
+                                </a:ext>
+                              </a:extLst>
+                            </xdr:cNvPr>
+                            <xdr:cNvSpPr txBox="1"/>
+                          </xdr:nvSpPr>
+                          <xdr:spPr>
+                            <a:xfrm>
+                              <a:off x="1837356" y="2882900"/>
+                              <a:ext cx="2870200" cy="2679700"/>
                             </a:xfrm>
                             <a:prstGeom prst="rect">
                               <a:avLst/>
@@ -1514,709 +1994,60 @@
                             <a:p>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000"/>
-                                <a:t>measurement	:</a:t>
+                                <a:t>rate:</a:t>
                               </a:r>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t> (</a:t>
+                                <a:t> String</a:t>
                               </a:r>
                             </a:p>
                             <a:p>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t>   weist: Number</a:t>
+                                <a:t>comment: String</a:t>
                               </a:r>
                             </a:p>
                             <a:p>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t>   bust: Number</a:t>
+                                <a:t>street: Sting</a:t>
                               </a:r>
                             </a:p>
                             <a:p>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t>   arm_length: Number</a:t>
+                                <a:t>clientId(FK)</a:t>
                               </a:r>
+                              <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
                             </a:p>
                             <a:p>
                               <a:r>
                                 <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t>   leg_length: Number</a:t>
-                              </a:r>
-                            </a:p>
-                            <a:p>
-                              <a:r>
-                                <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t>)</a:t>
-                              </a:r>
-                            </a:p>
-                            <a:p>
-                              <a:r>
-                                <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t>orders: FK(Array)</a:t>
-                              </a:r>
-                            </a:p>
-                            <a:p>
-                              <a:r>
-                                <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                <a:t>usersId: (FK)</a:t>
+                                <a:t>providerId(FK)</a:t>
                               </a:r>
                             </a:p>
                           </xdr:txBody>
                         </xdr:sp>
                       </xdr:grpSp>
-                      <xdr:grpSp>
-                        <xdr:nvGrpSpPr>
-                          <xdr:cNvPr id="59" name="Group 58">
+                      <xdr:cxnSp macro="">
+                        <xdr:nvCxnSpPr>
+                          <xdr:cNvPr id="48" name="Elbow Connector 47">
                             <a:extLst>
                               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE38A0E4-956E-8048-B6CF-6CB398E9DCB7}"/>
-                              </a:ext>
-                            </a:extLst>
-                          </xdr:cNvPr>
-                          <xdr:cNvGrpSpPr/>
-                        </xdr:nvGrpSpPr>
-                        <xdr:grpSpPr>
-                          <a:xfrm>
-                            <a:off x="9880600" y="1155700"/>
-                            <a:ext cx="5168901" cy="10312400"/>
-                            <a:chOff x="10363200" y="825500"/>
-                            <a:chExt cx="5168901" cy="10312400"/>
-                          </a:xfrm>
-                        </xdr:grpSpPr>
-                        <xdr:grpSp>
-                          <xdr:nvGrpSpPr>
-                            <xdr:cNvPr id="11" name="Group 10">
-                              <a:extLst>
-                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B9CF36B-7C68-0143-A73D-E8FA7F4DD114}"/>
-                                </a:ext>
-                              </a:extLst>
-                            </xdr:cNvPr>
-                            <xdr:cNvGrpSpPr/>
-                          </xdr:nvGrpSpPr>
-                          <xdr:grpSpPr>
-                            <a:xfrm>
-                              <a:off x="10363200" y="825500"/>
-                              <a:ext cx="3563513" cy="5702300"/>
-                              <a:chOff x="1562100" y="723900"/>
-                              <a:chExt cx="3563513" cy="5702300"/>
-                            </a:xfrm>
-                          </xdr:grpSpPr>
-                          <xdr:grpSp>
-                            <xdr:nvGrpSpPr>
-                              <xdr:cNvPr id="12" name="Group 11">
-                                <a:extLst>
-                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27402B51-87F8-F14A-984A-00F5F7BDB21D}"/>
-                                  </a:ext>
-                                </a:extLst>
-                              </xdr:cNvPr>
-                              <xdr:cNvGrpSpPr/>
-                            </xdr:nvGrpSpPr>
-                            <xdr:grpSpPr>
-                              <a:xfrm>
-                                <a:off x="1562100" y="723900"/>
-                                <a:ext cx="3563513" cy="5702300"/>
-                                <a:chOff x="1562100" y="723900"/>
-                                <a:chExt cx="3563513" cy="5702300"/>
-                              </a:xfrm>
-                            </xdr:grpSpPr>
-                            <xdr:sp macro="" textlink="">
-                              <xdr:nvSpPr>
-                                <xdr:cNvPr id="15" name="Process 14">
-                                  <a:extLst>
-                                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D869B504-945F-7B49-B644-07555770576A}"/>
-                                    </a:ext>
-                                  </a:extLst>
-                                </xdr:cNvPr>
-                                <xdr:cNvSpPr/>
-                              </xdr:nvSpPr>
-                              <xdr:spPr>
-                                <a:xfrm>
-                                  <a:off x="1587499" y="723900"/>
-                                  <a:ext cx="3505695" cy="5702300"/>
-                                </a:xfrm>
-                                <a:prstGeom prst="flowChartProcess">
-                                  <a:avLst/>
-                                </a:prstGeom>
-                              </xdr:spPr>
-                              <xdr:style>
-                                <a:lnRef idx="2">
-                                  <a:schemeClr val="accent6"/>
-                                </a:lnRef>
-                                <a:fillRef idx="1">
-                                  <a:schemeClr val="lt1"/>
-                                </a:fillRef>
-                                <a:effectRef idx="0">
-                                  <a:schemeClr val="accent6"/>
-                                </a:effectRef>
-                                <a:fontRef idx="minor">
-                                  <a:schemeClr val="dk1"/>
-                                </a:fontRef>
-                              </xdr:style>
-                              <xdr:txBody>
-                                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                                <a:lstStyle/>
-                                <a:p>
-                                  <a:pPr algn="l"/>
-                                  <a:endParaRPr lang="en-US" sz="1100"/>
-                                </a:p>
-                                <a:p>
-                                  <a:pPr algn="l"/>
-                                  <a:r>
-                                    <a:rPr lang="en-US" sz="1800"/>
-                                    <a:t>	</a:t>
-                                  </a:r>
-                                </a:p>
-                              </xdr:txBody>
-                            </xdr:sp>
-                            <xdr:cxnSp macro="">
-                              <xdr:nvCxnSpPr>
-                                <xdr:cNvPr id="16" name="Straight Connector 15">
-                                  <a:extLst>
-                                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7551C24-9DE9-134B-8100-BBACF07BBC9B}"/>
-                                    </a:ext>
-                                  </a:extLst>
-                                </xdr:cNvPr>
-                                <xdr:cNvCxnSpPr/>
-                              </xdr:nvCxnSpPr>
-                              <xdr:spPr>
-                                <a:xfrm>
-                                  <a:off x="1562100" y="1587500"/>
-                                  <a:ext cx="3563513" cy="29633"/>
-                                </a:xfrm>
-                                <a:prstGeom prst="line">
-                                  <a:avLst/>
-                                </a:prstGeom>
-                              </xdr:spPr>
-                              <xdr:style>
-                                <a:lnRef idx="1">
-                                  <a:schemeClr val="accent1"/>
-                                </a:lnRef>
-                                <a:fillRef idx="0">
-                                  <a:schemeClr val="accent1"/>
-                                </a:fillRef>
-                                <a:effectRef idx="0">
-                                  <a:schemeClr val="accent1"/>
-                                </a:effectRef>
-                                <a:fontRef idx="minor">
-                                  <a:schemeClr val="tx1"/>
-                                </a:fontRef>
-                              </xdr:style>
-                            </xdr:cxnSp>
-                          </xdr:grpSp>
-                          <xdr:sp macro="" textlink="">
-                            <xdr:nvSpPr>
-                              <xdr:cNvPr id="13" name="TextBox 12">
-                                <a:extLst>
-                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF912565-9D52-9044-9609-A04D56ECF7F7}"/>
-                                  </a:ext>
-                                </a:extLst>
-                              </xdr:cNvPr>
-                              <xdr:cNvSpPr txBox="1"/>
-                            </xdr:nvSpPr>
-                            <xdr:spPr>
-                              <a:xfrm>
-                                <a:off x="2298700" y="939800"/>
-                                <a:ext cx="2006600" cy="482600"/>
-                              </a:xfrm>
-                              <a:prstGeom prst="rect">
-                                <a:avLst/>
-                              </a:prstGeom>
-                              <a:solidFill>
-                                <a:schemeClr val="lt1"/>
-                              </a:solidFill>
-                              <a:ln w="9525" cmpd="sng">
-                                <a:solidFill>
-                                  <a:schemeClr val="lt1">
-                                    <a:shade val="50000"/>
-                                  </a:schemeClr>
-                                </a:solidFill>
-                              </a:ln>
-                            </xdr:spPr>
-                            <xdr:style>
-                              <a:lnRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:lnRef>
-                              <a:fillRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:fillRef>
-                              <a:effectRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:effectRef>
-                              <a:fontRef idx="minor">
-                                <a:schemeClr val="dk1"/>
-                              </a:fontRef>
-                            </xdr:style>
-                            <xdr:txBody>
-                              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-                              <a:lstStyle/>
-                              <a:p>
-                                <a:pPr algn="ctr"/>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2400"/>
-                                  <a:t>Providers</a:t>
-                                </a:r>
-                              </a:p>
-                            </xdr:txBody>
-                          </xdr:sp>
-                          <xdr:sp macro="" textlink="">
-                            <xdr:nvSpPr>
-                              <xdr:cNvPr id="14" name="TextBox 13">
-                                <a:extLst>
-                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F50ADC-0BA1-D944-AA3E-CA1B19225CC0}"/>
-                                  </a:ext>
-                                </a:extLst>
-                              </xdr:cNvPr>
-                              <xdr:cNvSpPr txBox="1"/>
-                            </xdr:nvSpPr>
-                            <xdr:spPr>
-                              <a:xfrm>
-                                <a:off x="1854200" y="1866899"/>
-                                <a:ext cx="3018738" cy="4389968"/>
-                              </a:xfrm>
-                              <a:prstGeom prst="rect">
-                                <a:avLst/>
-                              </a:prstGeom>
-                              <a:solidFill>
-                                <a:schemeClr val="lt1"/>
-                              </a:solidFill>
-                              <a:ln w="9525" cmpd="sng">
-                                <a:solidFill>
-                                  <a:schemeClr val="lt1">
-                                    <a:shade val="50000"/>
-                                  </a:schemeClr>
-                                </a:solidFill>
-                              </a:ln>
-                            </xdr:spPr>
-                            <xdr:style>
-                              <a:lnRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:lnRef>
-                              <a:fillRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:fillRef>
-                              <a:effectRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:effectRef>
-                              <a:fontRef idx="minor">
-                                <a:schemeClr val="dk1"/>
-                              </a:fontRef>
-                            </xdr:style>
-                            <xdr:txBody>
-                              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-                              <a:lstStyle/>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000"/>
-                                  <a:t>_id: Primary key </a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t>demo: String(web link)</a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t>photo: String(Web link)</a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t>category: String</a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000"/>
-                                  <a:t>orders: FK (Array)</a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000"/>
-                                  <a:t>userId(FK)</a:t>
-                                </a:r>
-                              </a:p>
-                            </xdr:txBody>
-                          </xdr:sp>
-                        </xdr:grpSp>
-                        <xdr:grpSp>
-                          <xdr:nvGrpSpPr>
-                            <xdr:cNvPr id="17" name="Group 16">
-                              <a:extLst>
-                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C078A5B-E556-E14B-ACDE-5386842E7585}"/>
-                                </a:ext>
-                              </a:extLst>
-                            </xdr:cNvPr>
-                            <xdr:cNvGrpSpPr/>
-                          </xdr:nvGrpSpPr>
-                          <xdr:grpSpPr>
-                            <a:xfrm>
-                              <a:off x="10473355" y="7023100"/>
-                              <a:ext cx="3352800" cy="4114800"/>
-                              <a:chOff x="1545255" y="1739900"/>
-                              <a:chExt cx="3352800" cy="4114800"/>
-                            </a:xfrm>
-                          </xdr:grpSpPr>
-                          <xdr:grpSp>
-                            <xdr:nvGrpSpPr>
-                              <xdr:cNvPr id="18" name="Group 17">
-                                <a:extLst>
-                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{550BD863-8F60-A34F-954F-643FF9ED6B08}"/>
-                                  </a:ext>
-                                </a:extLst>
-                              </xdr:cNvPr>
-                              <xdr:cNvGrpSpPr/>
-                            </xdr:nvGrpSpPr>
-                            <xdr:grpSpPr>
-                              <a:xfrm>
-                                <a:off x="1545255" y="1739900"/>
-                                <a:ext cx="3352800" cy="4114800"/>
-                                <a:chOff x="1545255" y="1739900"/>
-                                <a:chExt cx="3352800" cy="4114800"/>
-                              </a:xfrm>
-                            </xdr:grpSpPr>
-                            <xdr:sp macro="" textlink="">
-                              <xdr:nvSpPr>
-                                <xdr:cNvPr id="21" name="Process 20">
-                                  <a:extLst>
-                                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53172DB7-8D2A-4F4F-AD26-947E88B3F7BB}"/>
-                                    </a:ext>
-                                  </a:extLst>
-                                </xdr:cNvPr>
-                                <xdr:cNvSpPr/>
-                              </xdr:nvSpPr>
-                              <xdr:spPr>
-                                <a:xfrm>
-                                  <a:off x="1570655" y="1739900"/>
-                                  <a:ext cx="3314700" cy="4114800"/>
-                                </a:xfrm>
-                                <a:prstGeom prst="flowChartProcess">
-                                  <a:avLst/>
-                                </a:prstGeom>
-                              </xdr:spPr>
-                              <xdr:style>
-                                <a:lnRef idx="2">
-                                  <a:schemeClr val="accent6"/>
-                                </a:lnRef>
-                                <a:fillRef idx="1">
-                                  <a:schemeClr val="lt1"/>
-                                </a:fillRef>
-                                <a:effectRef idx="0">
-                                  <a:schemeClr val="accent6"/>
-                                </a:effectRef>
-                                <a:fontRef idx="minor">
-                                  <a:schemeClr val="dk1"/>
-                                </a:fontRef>
-                              </xdr:style>
-                              <xdr:txBody>
-                                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                                <a:lstStyle/>
-                                <a:p>
-                                  <a:pPr algn="l"/>
-                                  <a:endParaRPr lang="en-US" sz="1100"/>
-                                </a:p>
-                                <a:p>
-                                  <a:pPr algn="l"/>
-                                  <a:r>
-                                    <a:rPr lang="en-US" sz="1800"/>
-                                    <a:t>	</a:t>
-                                  </a:r>
-                                </a:p>
-                              </xdr:txBody>
-                            </xdr:sp>
-                            <xdr:cxnSp macro="">
-                              <xdr:nvCxnSpPr>
-                                <xdr:cNvPr id="22" name="Straight Connector 21">
-                                  <a:extLst>
-                                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61B48F51-0827-B242-852D-17948613BE1A}"/>
-                                    </a:ext>
-                                  </a:extLst>
-                                </xdr:cNvPr>
-                                <xdr:cNvCxnSpPr/>
-                              </xdr:nvCxnSpPr>
-                              <xdr:spPr>
-                                <a:xfrm>
-                                  <a:off x="1545255" y="2603500"/>
-                                  <a:ext cx="3352800" cy="0"/>
-                                </a:xfrm>
-                                <a:prstGeom prst="line">
-                                  <a:avLst/>
-                                </a:prstGeom>
-                              </xdr:spPr>
-                              <xdr:style>
-                                <a:lnRef idx="1">
-                                  <a:schemeClr val="accent1"/>
-                                </a:lnRef>
-                                <a:fillRef idx="0">
-                                  <a:schemeClr val="accent1"/>
-                                </a:fillRef>
-                                <a:effectRef idx="0">
-                                  <a:schemeClr val="accent1"/>
-                                </a:effectRef>
-                                <a:fontRef idx="minor">
-                                  <a:schemeClr val="tx1"/>
-                                </a:fontRef>
-                              </xdr:style>
-                            </xdr:cxnSp>
-                          </xdr:grpSp>
-                          <xdr:sp macro="" textlink="">
-                            <xdr:nvSpPr>
-                              <xdr:cNvPr id="19" name="TextBox 18">
-                                <a:extLst>
-                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF63E278-3D33-0E4B-A98E-2865211A52CF}"/>
-                                  </a:ext>
-                                </a:extLst>
-                              </xdr:cNvPr>
-                              <xdr:cNvSpPr txBox="1"/>
-                            </xdr:nvSpPr>
-                            <xdr:spPr>
-                              <a:xfrm>
-                                <a:off x="2281855" y="1955800"/>
-                                <a:ext cx="2006600" cy="482600"/>
-                              </a:xfrm>
-                              <a:prstGeom prst="rect">
-                                <a:avLst/>
-                              </a:prstGeom>
-                              <a:solidFill>
-                                <a:schemeClr val="lt1"/>
-                              </a:solidFill>
-                              <a:ln w="9525" cmpd="sng">
-                                <a:solidFill>
-                                  <a:schemeClr val="lt1">
-                                    <a:shade val="50000"/>
-                                  </a:schemeClr>
-                                </a:solidFill>
-                              </a:ln>
-                            </xdr:spPr>
-                            <xdr:style>
-                              <a:lnRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:lnRef>
-                              <a:fillRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:fillRef>
-                              <a:effectRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:effectRef>
-                              <a:fontRef idx="minor">
-                                <a:schemeClr val="dk1"/>
-                              </a:fontRef>
-                            </xdr:style>
-                            <xdr:txBody>
-                              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-                              <a:lstStyle/>
-                              <a:p>
-                                <a:pPr algn="ctr"/>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2400"/>
-                                  <a:t>Reviews</a:t>
-                                </a:r>
-                              </a:p>
-                            </xdr:txBody>
-                          </xdr:sp>
-                          <xdr:sp macro="" textlink="">
-                            <xdr:nvSpPr>
-                              <xdr:cNvPr id="20" name="TextBox 19">
-                                <a:extLst>
-                                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A50AE9-0294-2B4C-9FC2-2DBA40869262}"/>
-                                  </a:ext>
-                                </a:extLst>
-                              </xdr:cNvPr>
-                              <xdr:cNvSpPr txBox="1"/>
-                            </xdr:nvSpPr>
-                            <xdr:spPr>
-                              <a:xfrm>
-                                <a:off x="1837356" y="2882900"/>
-                                <a:ext cx="2870200" cy="2679700"/>
-                              </a:xfrm>
-                              <a:prstGeom prst="rect">
-                                <a:avLst/>
-                              </a:prstGeom>
-                              <a:solidFill>
-                                <a:schemeClr val="lt1"/>
-                              </a:solidFill>
-                              <a:ln w="9525" cmpd="sng">
-                                <a:solidFill>
-                                  <a:schemeClr val="lt1">
-                                    <a:shade val="50000"/>
-                                  </a:schemeClr>
-                                </a:solidFill>
-                              </a:ln>
-                            </xdr:spPr>
-                            <xdr:style>
-                              <a:lnRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:lnRef>
-                              <a:fillRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:fillRef>
-                              <a:effectRef idx="0">
-                                <a:scrgbClr r="0" g="0" b="0"/>
-                              </a:effectRef>
-                              <a:fontRef idx="minor">
-                                <a:schemeClr val="dk1"/>
-                              </a:fontRef>
-                            </xdr:style>
-                            <xdr:txBody>
-                              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-                              <a:lstStyle/>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000"/>
-                                  <a:t>_id: Primary key </a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000"/>
-                                  <a:t>rate:</a:t>
-                                </a:r>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t> String</a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t>comment: String</a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t>street: Sting</a:t>
-                                </a:r>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t>clientId(FK)</a:t>
-                                </a:r>
-                                <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-                              </a:p>
-                              <a:p>
-                                <a:r>
-                                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                                  <a:t>providerId(FK)</a:t>
-                                </a:r>
-                              </a:p>
-                            </xdr:txBody>
-                          </xdr:sp>
-                        </xdr:grpSp>
-                        <xdr:cxnSp macro="">
-                          <xdr:nvCxnSpPr>
-                            <xdr:cNvPr id="48" name="Elbow Connector 47">
-                              <a:extLst>
-                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EA3D42B-0DC5-E340-833C-F42D6B4FBE43}"/>
-                                </a:ext>
-                              </a:extLst>
-                            </xdr:cNvPr>
-                            <xdr:cNvCxnSpPr/>
-                          </xdr:nvCxnSpPr>
-                          <xdr:spPr>
-                            <a:xfrm rot="5400000">
-                              <a:off x="10161248" y="4560550"/>
-                              <a:ext cx="7670802" cy="3070905"/>
-                            </a:xfrm>
-                            <a:prstGeom prst="bentConnector3">
-                              <a:avLst>
-                                <a:gd name="adj1" fmla="val 100552"/>
-                              </a:avLst>
-                            </a:prstGeom>
-                            <a:ln>
-                              <a:tailEnd type="triangle"/>
-                            </a:ln>
-                          </xdr:spPr>
-                          <xdr:style>
-                            <a:lnRef idx="1">
-                              <a:schemeClr val="accent1"/>
-                            </a:lnRef>
-                            <a:fillRef idx="0">
-                              <a:schemeClr val="accent1"/>
-                            </a:fillRef>
-                            <a:effectRef idx="0">
-                              <a:schemeClr val="accent1"/>
-                            </a:effectRef>
-                            <a:fontRef idx="minor">
-                              <a:schemeClr val="tx1"/>
-                            </a:fontRef>
-                          </xdr:style>
-                        </xdr:cxnSp>
-                        <xdr:cxnSp macro="">
-                          <xdr:nvCxnSpPr>
-                            <xdr:cNvPr id="58" name="Straight Connector 57">
-                              <a:extLst>
-                                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33BC6F01-04E3-1243-B8F1-60D38C1399A1}"/>
-                                </a:ext>
-                              </a:extLst>
-                            </xdr:cNvPr>
-                            <xdr:cNvCxnSpPr/>
-                          </xdr:nvCxnSpPr>
-                          <xdr:spPr>
-                            <a:xfrm>
-                              <a:off x="12484100" y="2222500"/>
-                              <a:ext cx="3048000" cy="25400"/>
-                            </a:xfrm>
-                            <a:prstGeom prst="line">
-                              <a:avLst/>
-                            </a:prstGeom>
-                          </xdr:spPr>
-                          <xdr:style>
-                            <a:lnRef idx="1">
-                              <a:schemeClr val="accent1"/>
-                            </a:lnRef>
-                            <a:fillRef idx="0">
-                              <a:schemeClr val="accent1"/>
-                            </a:fillRef>
-                            <a:effectRef idx="0">
-                              <a:schemeClr val="accent1"/>
-                            </a:effectRef>
-                            <a:fontRef idx="minor">
-                              <a:schemeClr val="tx1"/>
-                            </a:fontRef>
-                          </xdr:style>
-                        </xdr:cxnSp>
-                      </xdr:grpSp>
-                      <xdr:cxnSp macro="">
-                        <xdr:nvCxnSpPr>
-                          <xdr:cNvPr id="64" name="Elbow Connector 63">
-                            <a:extLst>
-                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2CE91A3-CD2E-DD40-82DB-24ABE492E933}"/>
+                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EA3D42B-0DC5-E340-833C-F42D6B4FBE43}"/>
                               </a:ext>
                             </a:extLst>
                           </xdr:cNvPr>
                           <xdr:cNvCxnSpPr/>
                         </xdr:nvCxnSpPr>
                         <xdr:spPr>
-                          <a:xfrm rot="16200000" flipH="1">
-                            <a:off x="3095776" y="2708123"/>
-                            <a:ext cx="7907867" cy="6657219"/>
+                          <a:xfrm rot="5400000">
+                            <a:off x="11259315" y="5646885"/>
+                            <a:ext cx="5486402" cy="3082636"/>
                           </a:xfrm>
                           <a:prstGeom prst="bentConnector3">
                             <a:avLst>
-                              <a:gd name="adj1" fmla="val 85760"/>
+                              <a:gd name="adj1" fmla="val 99383"/>
                             </a:avLst>
                           </a:prstGeom>
                           <a:ln>
@@ -2238,13 +2069,48 @@
                           </a:fontRef>
                         </xdr:style>
                       </xdr:cxnSp>
+                      <xdr:cxnSp macro="">
+                        <xdr:nvCxnSpPr>
+                          <xdr:cNvPr id="58" name="Straight Connector 57">
+                            <a:extLst>
+                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33BC6F01-04E3-1243-B8F1-60D38C1399A1}"/>
+                              </a:ext>
+                            </a:extLst>
+                          </xdr:cNvPr>
+                          <xdr:cNvCxnSpPr/>
+                        </xdr:nvCxnSpPr>
+                        <xdr:spPr>
+                          <a:xfrm>
+                            <a:off x="8536306" y="3124200"/>
+                            <a:ext cx="7041218" cy="1303866"/>
+                          </a:xfrm>
+                          <a:prstGeom prst="line">
+                            <a:avLst/>
+                          </a:prstGeom>
+                        </xdr:spPr>
+                        <xdr:style>
+                          <a:lnRef idx="1">
+                            <a:schemeClr val="accent1"/>
+                          </a:lnRef>
+                          <a:fillRef idx="0">
+                            <a:schemeClr val="accent1"/>
+                          </a:fillRef>
+                          <a:effectRef idx="0">
+                            <a:schemeClr val="accent1"/>
+                          </a:effectRef>
+                          <a:fontRef idx="minor">
+                            <a:schemeClr val="tx1"/>
+                          </a:fontRef>
+                        </xdr:style>
+                      </xdr:cxnSp>
                     </xdr:grpSp>
                     <xdr:cxnSp macro="">
                       <xdr:nvCxnSpPr>
-                        <xdr:cNvPr id="89" name="Elbow Connector 88">
+                        <xdr:cNvPr id="64" name="Elbow Connector 63">
                           <a:extLst>
                             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19A0A1B-DD4C-5E4A-89DE-30E4BD701E4D}"/>
+                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2CE91A3-CD2E-DD40-82DB-24ABE492E933}"/>
                             </a:ext>
                           </a:extLst>
                         </xdr:cNvPr>
@@ -2252,12 +2118,12 @@
                       </xdr:nvCxnSpPr>
                       <xdr:spPr>
                         <a:xfrm rot="16200000" flipH="1">
-                          <a:off x="3359150" y="3930650"/>
-                          <a:ext cx="4229100" cy="609600"/>
+                          <a:off x="5948234" y="5560580"/>
+                          <a:ext cx="6400797" cy="2459373"/>
                         </a:xfrm>
                         <a:prstGeom prst="bentConnector3">
                           <a:avLst>
-                            <a:gd name="adj1" fmla="val 99550"/>
+                            <a:gd name="adj1" fmla="val 97884"/>
                           </a:avLst>
                         </a:prstGeom>
                         <a:ln>
@@ -2280,337 +2146,25 @@
                       </xdr:style>
                     </xdr:cxnSp>
                   </xdr:grpSp>
-                  <xdr:grpSp>
-                    <xdr:nvGrpSpPr>
-                      <xdr:cNvPr id="103" name="Group 102">
+                  <xdr:cxnSp macro="">
+                    <xdr:nvCxnSpPr>
+                      <xdr:cNvPr id="89" name="Elbow Connector 88">
                         <a:extLst>
                           <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1B13FE-68A6-E84D-8FB4-818BA09F455C}"/>
-                          </a:ext>
-                        </a:extLst>
-                      </xdr:cNvPr>
-                      <xdr:cNvGrpSpPr/>
-                    </xdr:nvGrpSpPr>
-                    <xdr:grpSpPr>
-                      <a:xfrm>
-                        <a:off x="3251200" y="9677399"/>
-                        <a:ext cx="3352800" cy="5020733"/>
-                        <a:chOff x="3251200" y="9677399"/>
-                        <a:chExt cx="3352800" cy="5020733"/>
-                      </a:xfrm>
-                    </xdr:grpSpPr>
-                    <xdr:grpSp>
-                      <xdr:nvGrpSpPr>
-                        <xdr:cNvPr id="100" name="Group 99">
-                          <a:extLst>
-                            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FBC651-E456-B541-B1C2-593FA57AB63B}"/>
-                            </a:ext>
-                          </a:extLst>
-                        </xdr:cNvPr>
-                        <xdr:cNvGrpSpPr/>
-                      </xdr:nvGrpSpPr>
-                      <xdr:grpSpPr>
-                        <a:xfrm>
-                          <a:off x="3251200" y="9677399"/>
-                          <a:ext cx="3352800" cy="5020733"/>
-                          <a:chOff x="3797300" y="1269999"/>
-                          <a:chExt cx="3352800" cy="5020733"/>
-                        </a:xfrm>
-                      </xdr:grpSpPr>
-                      <xdr:sp macro="" textlink="">
-                        <xdr:nvSpPr>
-                          <xdr:cNvPr id="98" name="Process 97">
-                            <a:extLst>
-                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E71F1336-B5F3-B54C-A245-61B2A65F0397}"/>
-                              </a:ext>
-                            </a:extLst>
-                          </xdr:cNvPr>
-                          <xdr:cNvSpPr/>
-                        </xdr:nvSpPr>
-                        <xdr:spPr>
-                          <a:xfrm>
-                            <a:off x="3822700" y="1269999"/>
-                            <a:ext cx="3314700" cy="5020733"/>
-                          </a:xfrm>
-                          <a:prstGeom prst="flowChartProcess">
-                            <a:avLst/>
-                          </a:prstGeom>
-                        </xdr:spPr>
-                        <xdr:style>
-                          <a:lnRef idx="2">
-                            <a:schemeClr val="accent6"/>
-                          </a:lnRef>
-                          <a:fillRef idx="1">
-                            <a:schemeClr val="lt1"/>
-                          </a:fillRef>
-                          <a:effectRef idx="0">
-                            <a:schemeClr val="accent6"/>
-                          </a:effectRef>
-                          <a:fontRef idx="minor">
-                            <a:schemeClr val="dk1"/>
-                          </a:fontRef>
-                        </xdr:style>
-                        <xdr:txBody>
-                          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                          <a:lstStyle/>
-                          <a:p>
-                            <a:pPr algn="l"/>
-                            <a:endParaRPr lang="en-US" sz="1100"/>
-                          </a:p>
-                          <a:p>
-                            <a:pPr algn="l"/>
-                            <a:r>
-                              <a:rPr lang="en-US" sz="1800"/>
-                              <a:t>	</a:t>
-                            </a:r>
-                          </a:p>
-                        </xdr:txBody>
-                      </xdr:sp>
-                      <xdr:cxnSp macro="">
-                        <xdr:nvCxnSpPr>
-                          <xdr:cNvPr id="99" name="Straight Connector 98">
-                            <a:extLst>
-                              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBB30EB-E87B-8A4C-B538-6968D42AAAA2}"/>
-                              </a:ext>
-                            </a:extLst>
-                          </xdr:cNvPr>
-                          <xdr:cNvCxnSpPr/>
-                        </xdr:nvCxnSpPr>
-                        <xdr:spPr>
-                          <a:xfrm>
-                            <a:off x="3797300" y="2133600"/>
-                            <a:ext cx="3352800" cy="0"/>
-                          </a:xfrm>
-                          <a:prstGeom prst="line">
-                            <a:avLst/>
-                          </a:prstGeom>
-                        </xdr:spPr>
-                        <xdr:style>
-                          <a:lnRef idx="1">
-                            <a:schemeClr val="accent1"/>
-                          </a:lnRef>
-                          <a:fillRef idx="0">
-                            <a:schemeClr val="accent1"/>
-                          </a:fillRef>
-                          <a:effectRef idx="0">
-                            <a:schemeClr val="accent1"/>
-                          </a:effectRef>
-                          <a:fontRef idx="minor">
-                            <a:schemeClr val="tx1"/>
-                          </a:fontRef>
-                        </xdr:style>
-                      </xdr:cxnSp>
-                    </xdr:grpSp>
-                    <xdr:sp macro="" textlink="">
-                      <xdr:nvSpPr>
-                        <xdr:cNvPr id="101" name="TextBox 100">
-                          <a:extLst>
-                            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48760D8D-A867-5541-BD90-22C624229AD4}"/>
-                            </a:ext>
-                          </a:extLst>
-                        </xdr:cNvPr>
-                        <xdr:cNvSpPr txBox="1"/>
-                      </xdr:nvSpPr>
-                      <xdr:spPr>
-                        <a:xfrm>
-                          <a:off x="3695700" y="9829800"/>
-                          <a:ext cx="2438400" cy="508000"/>
-                        </a:xfrm>
-                        <a:prstGeom prst="rect">
-                          <a:avLst/>
-                        </a:prstGeom>
-                        <a:solidFill>
-                          <a:schemeClr val="lt1"/>
-                        </a:solidFill>
-                        <a:ln w="9525" cmpd="sng">
-                          <a:solidFill>
-                            <a:schemeClr val="lt1">
-                              <a:shade val="50000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:ln>
-                      </xdr:spPr>
-                      <xdr:style>
-                        <a:lnRef idx="0">
-                          <a:scrgbClr r="0" g="0" b="0"/>
-                        </a:lnRef>
-                        <a:fillRef idx="0">
-                          <a:scrgbClr r="0" g="0" b="0"/>
-                        </a:fillRef>
-                        <a:effectRef idx="0">
-                          <a:scrgbClr r="0" g="0" b="0"/>
-                        </a:effectRef>
-                        <a:fontRef idx="minor">
-                          <a:schemeClr val="dk1"/>
-                        </a:fontRef>
-                      </xdr:style>
-                      <xdr:txBody>
-                        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-                        <a:lstStyle/>
-                        <a:p>
-                          <a:pPr algn="ctr"/>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>Orders</a:t>
-                          </a:r>
-                        </a:p>
-                      </xdr:txBody>
-                    </xdr:sp>
-                    <xdr:sp macro="" textlink="">
-                      <xdr:nvSpPr>
-                        <xdr:cNvPr id="102" name="TextBox 101">
-                          <a:extLst>
-                            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EA6B31F-82C0-4242-97E8-98BBFBE83059}"/>
-                            </a:ext>
-                          </a:extLst>
-                        </xdr:cNvPr>
-                        <xdr:cNvSpPr txBox="1"/>
-                      </xdr:nvSpPr>
-                      <xdr:spPr>
-                        <a:xfrm>
-                          <a:off x="3543300" y="10782299"/>
-                          <a:ext cx="2755900" cy="3627967"/>
-                        </a:xfrm>
-                        <a:prstGeom prst="rect">
-                          <a:avLst/>
-                        </a:prstGeom>
-                        <a:solidFill>
-                          <a:schemeClr val="lt1"/>
-                        </a:solidFill>
-                        <a:ln w="9525" cmpd="sng">
-                          <a:solidFill>
-                            <a:schemeClr val="lt1">
-                              <a:shade val="50000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:ln>
-                      </xdr:spPr>
-                      <xdr:style>
-                        <a:lnRef idx="0">
-                          <a:scrgbClr r="0" g="0" b="0"/>
-                        </a:lnRef>
-                        <a:fillRef idx="0">
-                          <a:scrgbClr r="0" g="0" b="0"/>
-                        </a:fillRef>
-                        <a:effectRef idx="0">
-                          <a:scrgbClr r="0" g="0" b="0"/>
-                        </a:effectRef>
-                        <a:fontRef idx="minor">
-                          <a:schemeClr val="dk1"/>
-                        </a:fontRef>
-                      </xdr:style>
-                      <xdr:txBody>
-                        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-                        <a:lstStyle/>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>_id: Primary Key</a:t>
-                          </a:r>
-                        </a:p>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>garment: garment(FK)</a:t>
-                          </a:r>
-                          <a:endParaRPr lang="en-US" sz="2000" baseline="0"/>
-                        </a:p>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                            <a:t>fablic: fabricId(FK)</a:t>
-                          </a:r>
-                        </a:p>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>budget: decimal</a:t>
-                          </a:r>
-                        </a:p>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>measurements: (</a:t>
-                          </a:r>
-                        </a:p>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                            <a:t>   </a:t>
-                          </a:r>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>weist: Number</a:t>
-                          </a:r>
-                          <a:br>
-                            <a:rPr lang="en-US" sz="2000"/>
-                          </a:br>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                            <a:t>    </a:t>
-                          </a:r>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>bust: Number</a:t>
-                          </a:r>
-                          <a:br>
-                            <a:rPr lang="en-US" sz="2000"/>
-                          </a:br>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                            <a:t>   </a:t>
-                          </a:r>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>arm_length: Number</a:t>
-                          </a:r>
-                          <a:br>
-                            <a:rPr lang="en-US" sz="2000"/>
-                          </a:br>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>leg_length: Number)</a:t>
-                          </a:r>
-                        </a:p>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>clientId(FK)</a:t>
-                          </a:r>
-                        </a:p>
-                        <a:p>
-                          <a:r>
-                            <a:rPr lang="en-US" sz="2000"/>
-                            <a:t>providerId(FK)</a:t>
-                          </a:r>
-                        </a:p>
-                      </xdr:txBody>
-                    </xdr:sp>
-                  </xdr:grpSp>
-                  <xdr:cxnSp macro="">
-                    <xdr:nvCxnSpPr>
-                      <xdr:cNvPr id="109" name="Elbow Connector 108">
-                        <a:extLst>
-                          <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B4958A-D0C9-7D49-A991-1CBCC55562A7}"/>
+                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19A0A1B-DD4C-5E4A-89DE-30E4BD701E4D}"/>
                           </a:ext>
                         </a:extLst>
                       </xdr:cNvPr>
                       <xdr:cNvCxnSpPr/>
                     </xdr:nvCxnSpPr>
                     <xdr:spPr>
-                      <a:xfrm rot="5400000" flipH="1" flipV="1">
-                        <a:off x="4362450" y="8096250"/>
-                        <a:ext cx="4089400" cy="1739900"/>
+                      <a:xfrm rot="16200000" flipH="1">
+                        <a:off x="3359150" y="3930650"/>
+                        <a:ext cx="4229100" cy="609600"/>
                       </a:xfrm>
                       <a:prstGeom prst="bentConnector3">
                         <a:avLst>
-                          <a:gd name="adj1" fmla="val -621"/>
+                          <a:gd name="adj1" fmla="val 99550"/>
                         </a:avLst>
                       </a:prstGeom>
                       <a:ln>
@@ -2633,25 +2187,292 @@
                     </xdr:style>
                   </xdr:cxnSp>
                 </xdr:grpSp>
+                <xdr:grpSp>
+                  <xdr:nvGrpSpPr>
+                    <xdr:cNvPr id="103" name="Group 102">
+                      <a:extLst>
+                        <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1B13FE-68A6-E84D-8FB4-818BA09F455C}"/>
+                        </a:ext>
+                      </a:extLst>
+                    </xdr:cNvPr>
+                    <xdr:cNvGrpSpPr/>
+                  </xdr:nvGrpSpPr>
+                  <xdr:grpSpPr>
+                    <a:xfrm>
+                      <a:off x="3251200" y="9677399"/>
+                      <a:ext cx="3352800" cy="5020733"/>
+                      <a:chOff x="3251200" y="9677399"/>
+                      <a:chExt cx="3352800" cy="5020733"/>
+                    </a:xfrm>
+                  </xdr:grpSpPr>
+                  <xdr:grpSp>
+                    <xdr:nvGrpSpPr>
+                      <xdr:cNvPr id="100" name="Group 99">
+                        <a:extLst>
+                          <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FBC651-E456-B541-B1C2-593FA57AB63B}"/>
+                          </a:ext>
+                        </a:extLst>
+                      </xdr:cNvPr>
+                      <xdr:cNvGrpSpPr/>
+                    </xdr:nvGrpSpPr>
+                    <xdr:grpSpPr>
+                      <a:xfrm>
+                        <a:off x="3251200" y="9677399"/>
+                        <a:ext cx="3352800" cy="5020733"/>
+                        <a:chOff x="3797300" y="1269999"/>
+                        <a:chExt cx="3352800" cy="5020733"/>
+                      </a:xfrm>
+                    </xdr:grpSpPr>
+                    <xdr:sp macro="" textlink="">
+                      <xdr:nvSpPr>
+                        <xdr:cNvPr id="98" name="Process 97">
+                          <a:extLst>
+                            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E71F1336-B5F3-B54C-A245-61B2A65F0397}"/>
+                            </a:ext>
+                          </a:extLst>
+                        </xdr:cNvPr>
+                        <xdr:cNvSpPr/>
+                      </xdr:nvSpPr>
+                      <xdr:spPr>
+                        <a:xfrm>
+                          <a:off x="3822700" y="1269999"/>
+                          <a:ext cx="3314700" cy="5020733"/>
+                        </a:xfrm>
+                        <a:prstGeom prst="flowChartProcess">
+                          <a:avLst/>
+                        </a:prstGeom>
+                      </xdr:spPr>
+                      <xdr:style>
+                        <a:lnRef idx="2">
+                          <a:schemeClr val="accent6"/>
+                        </a:lnRef>
+                        <a:fillRef idx="1">
+                          <a:schemeClr val="lt1"/>
+                        </a:fillRef>
+                        <a:effectRef idx="0">
+                          <a:schemeClr val="accent6"/>
+                        </a:effectRef>
+                        <a:fontRef idx="minor">
+                          <a:schemeClr val="dk1"/>
+                        </a:fontRef>
+                      </xdr:style>
+                      <xdr:txBody>
+                        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                        <a:lstStyle/>
+                        <a:p>
+                          <a:pPr algn="l"/>
+                          <a:endParaRPr lang="en-US" sz="1100"/>
+                        </a:p>
+                        <a:p>
+                          <a:pPr algn="l"/>
+                          <a:r>
+                            <a:rPr lang="en-US" sz="1800"/>
+                            <a:t>	</a:t>
+                          </a:r>
+                        </a:p>
+                      </xdr:txBody>
+                    </xdr:sp>
+                    <xdr:cxnSp macro="">
+                      <xdr:nvCxnSpPr>
+                        <xdr:cNvPr id="99" name="Straight Connector 98">
+                          <a:extLst>
+                            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CBB30EB-E87B-8A4C-B538-6968D42AAAA2}"/>
+                            </a:ext>
+                          </a:extLst>
+                        </xdr:cNvPr>
+                        <xdr:cNvCxnSpPr/>
+                      </xdr:nvCxnSpPr>
+                      <xdr:spPr>
+                        <a:xfrm>
+                          <a:off x="3797300" y="2133600"/>
+                          <a:ext cx="3352800" cy="0"/>
+                        </a:xfrm>
+                        <a:prstGeom prst="line">
+                          <a:avLst/>
+                        </a:prstGeom>
+                      </xdr:spPr>
+                      <xdr:style>
+                        <a:lnRef idx="1">
+                          <a:schemeClr val="accent1"/>
+                        </a:lnRef>
+                        <a:fillRef idx="0">
+                          <a:schemeClr val="accent1"/>
+                        </a:fillRef>
+                        <a:effectRef idx="0">
+                          <a:schemeClr val="accent1"/>
+                        </a:effectRef>
+                        <a:fontRef idx="minor">
+                          <a:schemeClr val="tx1"/>
+                        </a:fontRef>
+                      </xdr:style>
+                    </xdr:cxnSp>
+                  </xdr:grpSp>
+                  <xdr:sp macro="" textlink="">
+                    <xdr:nvSpPr>
+                      <xdr:cNvPr id="101" name="TextBox 100">
+                        <a:extLst>
+                          <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48760D8D-A867-5541-BD90-22C624229AD4}"/>
+                          </a:ext>
+                        </a:extLst>
+                      </xdr:cNvPr>
+                      <xdr:cNvSpPr txBox="1"/>
+                    </xdr:nvSpPr>
+                    <xdr:spPr>
+                      <a:xfrm>
+                        <a:off x="3695700" y="9829800"/>
+                        <a:ext cx="2438400" cy="508000"/>
+                      </a:xfrm>
+                      <a:prstGeom prst="rect">
+                        <a:avLst/>
+                      </a:prstGeom>
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:ln w="9525" cmpd="sng">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1">
+                            <a:shade val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:ln>
+                    </xdr:spPr>
+                    <xdr:style>
+                      <a:lnRef idx="0">
+                        <a:scrgbClr r="0" g="0" b="0"/>
+                      </a:lnRef>
+                      <a:fillRef idx="0">
+                        <a:scrgbClr r="0" g="0" b="0"/>
+                      </a:fillRef>
+                      <a:effectRef idx="0">
+                        <a:scrgbClr r="0" g="0" b="0"/>
+                      </a:effectRef>
+                      <a:fontRef idx="minor">
+                        <a:schemeClr val="dk1"/>
+                      </a:fontRef>
+                    </xdr:style>
+                    <xdr:txBody>
+                      <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:pPr algn="ctr"/>
+                        <a:r>
+                          <a:rPr lang="en-US" sz="2000"/>
+                          <a:t>Orders</a:t>
+                        </a:r>
+                      </a:p>
+                    </xdr:txBody>
+                  </xdr:sp>
+                  <xdr:sp macro="" textlink="">
+                    <xdr:nvSpPr>
+                      <xdr:cNvPr id="102" name="TextBox 101">
+                        <a:extLst>
+                          <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                            <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EA6B31F-82C0-4242-97E8-98BBFBE83059}"/>
+                          </a:ext>
+                        </a:extLst>
+                      </xdr:cNvPr>
+                      <xdr:cNvSpPr txBox="1"/>
+                    </xdr:nvSpPr>
+                    <xdr:spPr>
+                      <a:xfrm>
+                        <a:off x="3543300" y="10782299"/>
+                        <a:ext cx="2755900" cy="3627967"/>
+                      </a:xfrm>
+                      <a:prstGeom prst="rect">
+                        <a:avLst/>
+                      </a:prstGeom>
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:ln w="9525" cmpd="sng">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1">
+                            <a:shade val="50000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:ln>
+                    </xdr:spPr>
+                    <xdr:style>
+                      <a:lnRef idx="0">
+                        <a:scrgbClr r="0" g="0" b="0"/>
+                      </a:lnRef>
+                      <a:fillRef idx="0">
+                        <a:scrgbClr r="0" g="0" b="0"/>
+                      </a:fillRef>
+                      <a:effectRef idx="0">
+                        <a:scrgbClr r="0" g="0" b="0"/>
+                      </a:effectRef>
+                      <a:fontRef idx="minor">
+                        <a:schemeClr val="dk1"/>
+                      </a:fontRef>
+                    </xdr:style>
+                    <xdr:txBody>
+                      <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+                      <a:lstStyle/>
+                      <a:p>
+                        <a:r>
+                          <a:rPr lang="en-US" sz="2000"/>
+                          <a:t>_id: Primary Key</a:t>
+                        </a:r>
+                      </a:p>
+                      <a:p>
+                        <a:r>
+                          <a:rPr lang="en-US" sz="2000"/>
+                          <a:t>garment: garment(FK)</a:t>
+                        </a:r>
+                        <a:endParaRPr lang="en-US" sz="2000" baseline="0"/>
+                      </a:p>
+                      <a:p>
+                        <a:r>
+                          <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                          <a:t>fablic: fabricId(FK)</a:t>
+                        </a:r>
+                      </a:p>
+                      <a:p>
+                        <a:r>
+                          <a:rPr lang="en-US" sz="2000"/>
+                          <a:t>budget: decimal</a:t>
+                        </a:r>
+                      </a:p>
+                      <a:p>
+                        <a:r>
+                          <a:rPr lang="en-US" sz="2000"/>
+                          <a:t>clientId(FK)(userId)</a:t>
+                        </a:r>
+                      </a:p>
+                      <a:p>
+                        <a:r>
+                          <a:rPr lang="en-US" sz="2000"/>
+                          <a:t>providerId(FK)(userId)</a:t>
+                        </a:r>
+                      </a:p>
+                    </xdr:txBody>
+                  </xdr:sp>
+                </xdr:grpSp>
                 <xdr:cxnSp macro="">
                   <xdr:nvCxnSpPr>
-                    <xdr:cNvPr id="116" name="Elbow Connector 115">
+                    <xdr:cNvPr id="109" name="Elbow Connector 108">
                       <a:extLst>
                         <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40B69F38-DEC8-404C-91F2-F4CE23410070}"/>
+                          <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B4958A-D0C9-7D49-A991-1CBCC55562A7}"/>
                         </a:ext>
                       </a:extLst>
                     </xdr:cNvPr>
                     <xdr:cNvCxnSpPr/>
                   </xdr:nvCxnSpPr>
                   <xdr:spPr>
-                    <a:xfrm rot="10800000" flipV="1">
-                      <a:off x="5585881" y="6333067"/>
-                      <a:ext cx="9963859" cy="4673600"/>
+                    <a:xfrm rot="5400000" flipH="1" flipV="1">
+                      <a:off x="3287121" y="5856879"/>
+                      <a:ext cx="7404101" cy="2903941"/>
                     </a:xfrm>
                     <a:prstGeom prst="bentConnector3">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -10862"/>
+                        <a:gd name="adj1" fmla="val 31704"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:ln>
@@ -2734,46 +2555,6 @@
                 <a:prstGeom prst="line">
                   <a:avLst/>
                 </a:prstGeom>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="1">
-                  <a:schemeClr val="accent1"/>
-                </a:lnRef>
-                <a:fillRef idx="0">
-                  <a:schemeClr val="accent1"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:schemeClr val="accent1"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="tx1"/>
-                </a:fontRef>
-              </xdr:style>
-            </xdr:cxnSp>
-            <xdr:cxnSp macro="">
-              <xdr:nvCxnSpPr>
-                <xdr:cNvPr id="136" name="Elbow Connector 135">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77F415C7-E03B-594C-802A-384E7A7CECB5}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvCxnSpPr/>
-              </xdr:nvCxnSpPr>
-              <xdr:spPr>
-                <a:xfrm rot="16200000" flipH="1">
-                  <a:off x="-1981323" y="6654854"/>
-                  <a:ext cx="7924804" cy="3251092"/>
-                </a:xfrm>
-                <a:prstGeom prst="bentConnector3">
-                  <a:avLst>
-                    <a:gd name="adj1" fmla="val 102991"/>
-                  </a:avLst>
-                </a:prstGeom>
-                <a:ln>
-                  <a:tailEnd type="triangle"/>
-                </a:ln>
               </xdr:spPr>
               <xdr:style>
                 <a:lnRef idx="1">
@@ -3276,16 +3057,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>186266</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>474133</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>389467</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>118533</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3299,9 +3080,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9313333" y="2523067"/>
-          <a:ext cx="1032934" cy="33866"/>
+        <a:xfrm flipH="1">
+          <a:off x="7941733" y="2827867"/>
+          <a:ext cx="1439334" cy="33866"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3326,16 +3107,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>491066</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152396</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>220134</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>186270</xdr:rowOff>
+      <xdr:colOff>237067</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>118537</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3350,12 +3131,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1185330" y="6045199"/>
-          <a:ext cx="11616274" cy="4707468"/>
+          <a:off x="2997199" y="3911601"/>
+          <a:ext cx="7450670" cy="5283201"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 124490"/>
+            <a:gd name="adj1" fmla="val 59773"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -3678,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908D1B3D-6ACC-E748-A087-A577BDF2B46B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>